<commit_message>
New Entry From Eclipse
</commit_message>
<xml_diff>
--- a/iConnectX/bin/Control_Data/Control_File.xlsx
+++ b/iConnectX/bin/Control_Data/Control_File.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Scenario_Id</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Upload_New_Photo</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>iCX_1</t>
@@ -411,7 +408,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,30 +435,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>